<commit_message>
embed backpack system with new UI system
</commit_message>
<xml_diff>
--- a/Luban/Config/Datas/Config.xlsx
+++ b/Luban/Config/Datas/Config.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowHeight="17940" activeTab="1"/>
+    <workbookView windowWidth="28125" windowHeight="12540"/>
   </bookViews>
   <sheets>
     <sheet name="UIConfig" sheetId="1" r:id="rId1"/>
@@ -80,7 +80,7 @@
     <t>UI_Dialog</t>
   </si>
   <si>
-    <t>UI_Inventory</t>
+    <t>UI_Backpack</t>
   </si>
   <si>
     <t>实体编号</t>
@@ -1102,8 +1102,8 @@
   <sheetPr/>
   <dimension ref="A1:F9"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1:F9"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="24" customHeight="1" outlineLevelCol="5"/>
@@ -1282,8 +1282,8 @@
   <sheetPr/>
   <dimension ref="A1:F7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="16.875" defaultRowHeight="28" customHeight="1" outlineLevelRow="6" outlineLevelCol="5"/>

</xml_diff>

<commit_message>
Auto stash before merge of "dev" and "origin/dev"
</commit_message>
<xml_diff>
--- a/Luban/Config/Datas/Config.xlsx
+++ b/Luban/Config/Datas/Config.xlsx
@@ -1,10 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="25601"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\GameDev\Blues-Dusk\Luban\Config\Datas\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{90D5C210-8809-41A8-B457-572BEC4B3911}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView windowWidth="28125" windowHeight="12540" activeTab="2"/>
+    <workbookView xWindow="-23148" yWindow="5304" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="UIConfig" sheetId="1" r:id="rId1"/>
@@ -16,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="34">
   <si>
     <t>##var</t>
   </si>
@@ -112,19 +118,21 @@
   </si>
   <si>
     <t>current_week</t>
+  </si>
+  <si>
+    <t>UI_GameMenu</t>
+    <phoneticPr fontId="8" type="noConversion"/>
+  </si>
+  <si>
+    <t>Default</t>
+    <phoneticPr fontId="8" type="noConversion"/>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="4">
-    <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
-  </numFmts>
-  <fonts count="25">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="11" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -136,7 +144,7 @@
       <sz val="12"/>
       <color rgb="FF24292F"/>
       <name val="Segoe UI"/>
-      <charset val="134"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="11"/>
@@ -167,150 +175,41 @@
     </font>
     <font>
       <sz val="11"/>
-      <color theme="1"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
       <color rgb="FF9C0006"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
       <name val="宋体"/>
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
+      <color rgb="FF006100"/>
       <name val="宋体"/>
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
+      <sz val="9"/>
       <name val="宋体"/>
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="宋体"/>
+      <family val="3"/>
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
+      <sz val="9"/>
       <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="宋体"/>
-      <charset val="0"/>
+      <family val="3"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="36">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -347,182 +246,8 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
   </fills>
-  <borders count="10">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -545,255 +270,19 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="double">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
-  <cellStyleXfs count="49">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="8" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="3" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="15" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="15" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="16" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -815,11 +304,11 @@
     <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="31" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="7" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="3" fontId="1" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -832,66 +321,27 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="1" xfId="31" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="31" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="4" fillId="6" borderId="1" xfId="7" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="7" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="1" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1">
+      <alignment vertical="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="49">
+  <cellStyles count="3">
+    <cellStyle name="差" xfId="1" builtinId="27"/>
     <cellStyle name="常规" xfId="0" builtinId="0"/>
-    <cellStyle name="货币[0]" xfId="1" builtinId="7"/>
-    <cellStyle name="20% - 强调文字颜色 3" xfId="2" builtinId="38"/>
-    <cellStyle name="输入" xfId="3" builtinId="20"/>
-    <cellStyle name="货币" xfId="4" builtinId="4"/>
-    <cellStyle name="千位分隔[0]" xfId="5" builtinId="6"/>
-    <cellStyle name="40% - 强调文字颜色 3" xfId="6" builtinId="39"/>
-    <cellStyle name="差" xfId="7" builtinId="27"/>
-    <cellStyle name="千位分隔" xfId="8" builtinId="3"/>
-    <cellStyle name="60% - 强调文字颜色 3" xfId="9" builtinId="40"/>
-    <cellStyle name="超链接" xfId="10" builtinId="8"/>
-    <cellStyle name="百分比" xfId="11" builtinId="5"/>
-    <cellStyle name="已访问的超链接" xfId="12" builtinId="9"/>
-    <cellStyle name="注释" xfId="13" builtinId="10"/>
-    <cellStyle name="60% - 强调文字颜色 2" xfId="14" builtinId="36"/>
-    <cellStyle name="标题 4" xfId="15" builtinId="19"/>
-    <cellStyle name="警告文本" xfId="16" builtinId="11"/>
-    <cellStyle name="标题" xfId="17" builtinId="15"/>
-    <cellStyle name="解释性文本" xfId="18" builtinId="53"/>
-    <cellStyle name="标题 1" xfId="19" builtinId="16"/>
-    <cellStyle name="标题 2" xfId="20" builtinId="17"/>
-    <cellStyle name="60% - 强调文字颜色 1" xfId="21" builtinId="32"/>
-    <cellStyle name="标题 3" xfId="22" builtinId="18"/>
-    <cellStyle name="60% - 强调文字颜色 4" xfId="23" builtinId="44"/>
-    <cellStyle name="输出" xfId="24" builtinId="21"/>
-    <cellStyle name="计算" xfId="25" builtinId="22"/>
-    <cellStyle name="检查单元格" xfId="26" builtinId="23"/>
-    <cellStyle name="20% - 强调文字颜色 6" xfId="27" builtinId="50"/>
-    <cellStyle name="强调文字颜色 2" xfId="28" builtinId="33"/>
-    <cellStyle name="链接单元格" xfId="29" builtinId="24"/>
-    <cellStyle name="汇总" xfId="30" builtinId="25"/>
-    <cellStyle name="好" xfId="31" builtinId="26"/>
-    <cellStyle name="适中" xfId="32" builtinId="28"/>
-    <cellStyle name="20% - 强调文字颜色 5" xfId="33" builtinId="46"/>
-    <cellStyle name="强调文字颜色 1" xfId="34" builtinId="29"/>
-    <cellStyle name="20% - 强调文字颜色 1" xfId="35" builtinId="30"/>
-    <cellStyle name="40% - 强调文字颜色 1" xfId="36" builtinId="31"/>
-    <cellStyle name="20% - 强调文字颜色 2" xfId="37" builtinId="34"/>
-    <cellStyle name="40% - 强调文字颜色 2" xfId="38" builtinId="35"/>
-    <cellStyle name="强调文字颜色 3" xfId="39" builtinId="37"/>
-    <cellStyle name="强调文字颜色 4" xfId="40" builtinId="41"/>
-    <cellStyle name="20% - 强调文字颜色 4" xfId="41" builtinId="42"/>
-    <cellStyle name="40% - 强调文字颜色 4" xfId="42" builtinId="43"/>
-    <cellStyle name="强调文字颜色 5" xfId="43" builtinId="45"/>
-    <cellStyle name="40% - 强调文字颜色 5" xfId="44" builtinId="47"/>
-    <cellStyle name="60% - 强调文字颜色 5" xfId="45" builtinId="48"/>
-    <cellStyle name="强调文字颜色 6" xfId="46" builtinId="49"/>
-    <cellStyle name="40% - 强调文字颜色 6" xfId="47" builtinId="51"/>
-    <cellStyle name="60% - 强调文字颜色 6" xfId="48" builtinId="52"/>
+    <cellStyle name="好" xfId="2" builtinId="26"/>
   </cellStyles>
+  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -1178,28 +628,28 @@
     </a:fmtScheme>
   </a:themeElements>
   <a:objectDefaults/>
+  <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
-  <sheetPr/>
-  <dimension ref="A1:F9"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:F10"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E13" sqref="E13"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G10" sqref="G10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="24" customHeight="1" outlineLevelCol="5"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="24" customHeight="1" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="20" customWidth="1"/>
-    <col min="2" max="4" width="15.875" customWidth="1"/>
-    <col min="5" max="5" width="29.5" customWidth="1"/>
-    <col min="6" max="6" width="44.125" customWidth="1"/>
-    <col min="7" max="7" width="27.375" customWidth="1"/>
+    <col min="2" max="4" width="15.86328125" customWidth="1"/>
+    <col min="5" max="5" width="29.46484375" customWidth="1"/>
+    <col min="6" max="6" width="44.1328125" customWidth="1"/>
+    <col min="7" max="7" width="27.3984375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" customHeight="1" spans="1:6">
+    <row r="1" spans="1:6" ht="24" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="14" t="s">
         <v>0</v>
       </c>
@@ -1219,7 +669,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" customHeight="1" spans="1:6">
+    <row r="2" spans="1:6" ht="24" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="14" t="s">
         <v>0</v>
       </c>
@@ -1229,7 +679,7 @@
       <c r="E2" s="14"/>
       <c r="F2" s="14"/>
     </row>
-    <row r="3" customHeight="1" spans="1:6">
+    <row r="3" spans="1:6" ht="24" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="16" t="s">
         <v>6</v>
       </c>
@@ -1249,7 +699,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="4" customHeight="1" spans="1:6">
+    <row r="4" spans="1:6" ht="24" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="14" t="s">
         <v>10</v>
       </c>
@@ -1269,7 +719,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="5" customHeight="1" spans="2:6">
+    <row r="5" spans="1:6" ht="24" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B5">
         <v>100</v>
       </c>
@@ -1286,7 +736,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" customHeight="1" spans="2:6">
+    <row r="6" spans="1:6" ht="24" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B6">
         <v>101</v>
       </c>
@@ -1303,7 +753,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" customHeight="1" spans="2:6">
+    <row r="7" spans="1:6" ht="24" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B7">
         <v>102</v>
       </c>
@@ -1320,7 +770,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" customHeight="1" spans="2:6">
+    <row r="8" spans="1:6" ht="24" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B8">
         <v>1000</v>
       </c>
@@ -1337,7 +787,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" customHeight="1" spans="2:6">
+    <row r="9" spans="1:6" ht="24" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B9">
         <v>1001</v>
       </c>
@@ -1354,31 +804,47 @@
         <v>1</v>
       </c>
     </row>
+    <row r="10" spans="1:6" ht="24" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B10">
+        <v>1002</v>
+      </c>
+      <c r="C10" s="18" t="s">
+        <v>32</v>
+      </c>
+      <c r="D10" s="18" t="s">
+        <v>33</v>
+      </c>
+      <c r="E10" t="b">
+        <v>0</v>
+      </c>
+      <c r="F10" t="b">
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
+  <phoneticPr fontId="8" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait"/>
-  <headerFooter/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
-  <sheetPr/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:F7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="16.875" defaultRowHeight="28" customHeight="1" outlineLevelRow="6" outlineLevelCol="5"/>
+  <sheetFormatPr defaultColWidth="16.86328125" defaultRowHeight="28.05" customHeight="1" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="4" width="16.875" customWidth="1"/>
-    <col min="5" max="5" width="26.875" customWidth="1"/>
-    <col min="6" max="6" width="25.375" customWidth="1"/>
-    <col min="7" max="16384" width="16.875" customWidth="1"/>
+    <col min="1" max="4" width="16.86328125" customWidth="1"/>
+    <col min="5" max="5" width="26.86328125" customWidth="1"/>
+    <col min="6" max="6" width="25.3984375" customWidth="1"/>
+    <col min="7" max="7" width="16.86328125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" customHeight="1" spans="1:6">
+    <row r="1" spans="1:6" ht="28.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="14" t="s">
         <v>0</v>
       </c>
@@ -1392,7 +858,7 @@
       <c r="E1" s="15"/>
       <c r="F1" s="15"/>
     </row>
-    <row r="2" customHeight="1" spans="1:6">
+    <row r="2" spans="1:6" ht="28.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="14" t="s">
         <v>0</v>
       </c>
@@ -1402,7 +868,7 @@
       <c r="E2" s="15"/>
       <c r="F2" s="15"/>
     </row>
-    <row r="3" customHeight="1" spans="1:6">
+    <row r="3" spans="1:6" ht="28.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="16" t="s">
         <v>6</v>
       </c>
@@ -1416,7 +882,7 @@
       <c r="E3" s="17"/>
       <c r="F3" s="17"/>
     </row>
-    <row r="4" customHeight="1" spans="1:6">
+    <row r="4" spans="1:6" ht="28.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="14" t="s">
         <v>10</v>
       </c>
@@ -1430,7 +896,7 @@
       <c r="E4" s="15"/>
       <c r="F4" s="15"/>
     </row>
-    <row r="5" customHeight="1" spans="2:3">
+    <row r="5" spans="1:6" ht="28.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B5">
         <v>10000</v>
       </c>
@@ -1438,7 +904,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="6" customHeight="1" spans="2:3">
+    <row r="6" spans="1:6" ht="28.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B6">
         <v>10001</v>
       </c>
@@ -1446,7 +912,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="7" customHeight="1" spans="2:3">
+    <row r="7" spans="1:6" ht="28.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B7">
         <v>10002</v>
       </c>
@@ -1455,33 +921,32 @@
       </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="10" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait"/>
-  <headerFooter/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
-  <sheetPr/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:F25"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="24" customHeight="1" outlineLevelCol="5"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="24" customHeight="1" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="20" style="1" customWidth="1"/>
-    <col min="2" max="2" width="15.875" style="2" customWidth="1"/>
-    <col min="3" max="3" width="19.75" style="3" customWidth="1"/>
-    <col min="4" max="4" width="15.875" style="3" customWidth="1"/>
-    <col min="5" max="5" width="29.5" customWidth="1"/>
-    <col min="6" max="6" width="44.125" customWidth="1"/>
-    <col min="7" max="7" width="27.375" customWidth="1"/>
+    <col min="2" max="2" width="15.86328125" style="2" customWidth="1"/>
+    <col min="3" max="3" width="19.73046875" style="3" customWidth="1"/>
+    <col min="4" max="4" width="15.86328125" style="3" customWidth="1"/>
+    <col min="5" max="5" width="29.46484375" customWidth="1"/>
+    <col min="6" max="6" width="44.1328125" customWidth="1"/>
+    <col min="7" max="7" width="27.3984375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="1" customHeight="1" spans="1:6">
+    <row r="1" spans="1:6" ht="24" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="4" t="s">
         <v>26</v>
       </c>
@@ -1495,7 +960,7 @@
       <c r="E1" s="7"/>
       <c r="F1" s="7"/>
     </row>
-    <row r="2" customFormat="1" customHeight="1" spans="1:6">
+    <row r="2" spans="1:6" ht="24" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="4" t="s">
         <v>27</v>
       </c>
@@ -1509,7 +974,7 @@
       <c r="E2" s="7"/>
       <c r="F2" s="7"/>
     </row>
-    <row r="3" customFormat="1" customHeight="1" spans="1:6">
+    <row r="3" spans="1:6" ht="24" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="4" t="s">
         <v>28</v>
       </c>
@@ -1523,7 +988,7 @@
       <c r="E3" s="9"/>
       <c r="F3" s="9"/>
     </row>
-    <row r="4" customFormat="1" customHeight="1" spans="1:6">
+    <row r="4" spans="1:6" ht="24" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="4" t="s">
         <v>29</v>
       </c>
@@ -1537,7 +1002,7 @@
       <c r="E4" s="7"/>
       <c r="F4" s="7"/>
     </row>
-    <row r="5" customFormat="1" customHeight="1" spans="1:4">
+    <row r="5" spans="1:6" ht="24" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="4" t="s">
         <v>30</v>
       </c>
@@ -1549,7 +1014,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" customFormat="1" customHeight="1" spans="1:4">
+    <row r="6" spans="1:6" ht="24" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="4" t="s">
         <v>31</v>
       </c>
@@ -1561,122 +1026,122 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" customFormat="1" customHeight="1" spans="1:4">
+    <row r="7" spans="1:6" ht="24" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="12"/>
       <c r="B7" s="13"/>
       <c r="C7" s="11"/>
       <c r="D7" s="11"/>
     </row>
-    <row r="8" customFormat="1" customHeight="1" spans="1:4">
+    <row r="8" spans="1:6" ht="24" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="12"/>
       <c r="B8" s="13"/>
       <c r="C8" s="11"/>
       <c r="D8" s="11"/>
     </row>
-    <row r="9" customFormat="1" customHeight="1" spans="1:4">
+    <row r="9" spans="1:6" ht="24" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="12"/>
       <c r="B9" s="13"/>
       <c r="C9" s="11"/>
       <c r="D9" s="11"/>
     </row>
-    <row r="10" customFormat="1" customHeight="1" spans="1:4">
+    <row r="10" spans="1:6" ht="24" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="12"/>
       <c r="B10" s="13"/>
       <c r="C10" s="11"/>
       <c r="D10" s="11"/>
     </row>
-    <row r="11" customFormat="1" customHeight="1" spans="1:4">
+    <row r="11" spans="1:6" ht="24" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" s="12"/>
       <c r="B11" s="13"/>
       <c r="C11" s="11"/>
       <c r="D11" s="11"/>
     </row>
-    <row r="12" customFormat="1" customHeight="1" spans="1:4">
+    <row r="12" spans="1:6" ht="24" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A12" s="12"/>
       <c r="B12" s="13"/>
       <c r="C12" s="11"/>
       <c r="D12" s="11"/>
     </row>
-    <row r="13" customFormat="1" customHeight="1" spans="1:4">
+    <row r="13" spans="1:6" ht="24" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A13" s="12"/>
       <c r="B13" s="13"/>
       <c r="C13" s="11"/>
       <c r="D13" s="11"/>
     </row>
-    <row r="14" customFormat="1" customHeight="1" spans="1:4">
+    <row r="14" spans="1:6" ht="24" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A14" s="12"/>
       <c r="B14" s="13"/>
       <c r="C14" s="11"/>
       <c r="D14" s="11"/>
     </row>
-    <row r="15" customFormat="1" customHeight="1" spans="1:4">
+    <row r="15" spans="1:6" ht="24" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A15" s="12"/>
       <c r="B15" s="13"/>
       <c r="C15" s="11"/>
       <c r="D15" s="11"/>
     </row>
-    <row r="16" customFormat="1" customHeight="1" spans="1:4">
+    <row r="16" spans="1:6" ht="24" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A16" s="12"/>
       <c r="B16" s="13"/>
       <c r="C16" s="11"/>
       <c r="D16" s="11"/>
     </row>
-    <row r="17" customFormat="1" customHeight="1" spans="1:4">
+    <row r="17" spans="1:4" ht="24" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A17" s="12"/>
       <c r="B17" s="13"/>
       <c r="C17" s="11"/>
       <c r="D17" s="11"/>
     </row>
-    <row r="18" customFormat="1" customHeight="1" spans="1:4">
+    <row r="18" spans="1:4" ht="24" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A18" s="12"/>
       <c r="B18" s="13"/>
       <c r="C18" s="11"/>
       <c r="D18" s="11"/>
     </row>
-    <row r="19" customFormat="1" customHeight="1" spans="1:4">
+    <row r="19" spans="1:4" ht="24" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A19" s="12"/>
       <c r="B19" s="13"/>
       <c r="C19" s="11"/>
       <c r="D19" s="11"/>
     </row>
-    <row r="20" customFormat="1" customHeight="1" spans="1:4">
+    <row r="20" spans="1:4" ht="24" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A20" s="12"/>
       <c r="B20" s="13"/>
       <c r="C20" s="11"/>
       <c r="D20" s="11"/>
     </row>
-    <row r="21" customFormat="1" customHeight="1" spans="1:4">
+    <row r="21" spans="1:4" ht="24" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A21" s="12"/>
       <c r="B21" s="13"/>
       <c r="C21" s="11"/>
       <c r="D21" s="11"/>
     </row>
-    <row r="22" customFormat="1" customHeight="1" spans="1:4">
+    <row r="22" spans="1:4" ht="24" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A22" s="12"/>
       <c r="B22" s="13"/>
       <c r="C22" s="11"/>
       <c r="D22" s="11"/>
     </row>
-    <row r="23" customFormat="1" customHeight="1" spans="1:4">
+    <row r="23" spans="1:4" ht="24" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A23" s="12"/>
       <c r="B23" s="13"/>
       <c r="C23" s="11"/>
       <c r="D23" s="11"/>
     </row>
-    <row r="24" customFormat="1" customHeight="1" spans="1:4">
+    <row r="24" spans="1:4" ht="24" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A24" s="12"/>
       <c r="B24" s="13"/>
       <c r="C24" s="11"/>
       <c r="D24" s="11"/>
     </row>
-    <row r="25" customFormat="1" customHeight="1" spans="1:4">
+    <row r="25" spans="1:4" ht="24" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A25" s="12"/>
       <c r="B25" s="13"/>
       <c r="C25" s="11"/>
       <c r="D25" s="11"/>
     </row>
   </sheetData>
+  <phoneticPr fontId="10" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <headerFooter/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
update Tip and SelectScene
</commit_message>
<xml_diff>
--- a/Luban/Config/Datas/Config.xlsx
+++ b/Luban/Config/Datas/Config.xlsx
@@ -1,28 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="25601"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\GameDev\Blues-Dusk\Luban\Config\Datas\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{90D5C210-8809-41A8-B457-572BEC4B3911}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-23148" yWindow="5304" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView windowWidth="28125" windowHeight="12540" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="UIConfig" sheetId="1" r:id="rId1"/>
     <sheet name="EntityConfig" sheetId="2" r:id="rId2"/>
     <sheet name="GameConfig" sheetId="3" r:id="rId3"/>
+    <sheet name="SceneConfig" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="144525"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="42">
   <si>
     <t>##var</t>
   </si>
@@ -90,6 +85,9 @@
     <t>UI_Backpack</t>
   </si>
   <si>
+    <t>UI_GameMenu</t>
+  </si>
+  <si>
     <t>实体编号</t>
   </si>
   <si>
@@ -120,22 +118,61 @@
     <t>current_week</t>
   </si>
   <si>
-    <t>UI_GameMenu</t>
-    <phoneticPr fontId="8" type="noConversion"/>
-  </si>
-  <si>
-    <t>Default</t>
-    <phoneticPr fontId="8" type="noConversion"/>
+    <t>scene_asset_name</t>
+  </si>
+  <si>
+    <t>is_unlock</t>
+  </si>
+  <si>
+    <t>场景资源名</t>
+  </si>
+  <si>
+    <t>是否解锁</t>
+  </si>
+  <si>
+    <t>S_Tower</t>
+  </si>
+  <si>
+    <t>S_Parlor</t>
+  </si>
+  <si>
+    <t>S_FengHospital</t>
+  </si>
+  <si>
+    <t>S_Station</t>
+  </si>
+  <si>
+    <t>S_Bar</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="11" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <numFmts count="4">
+    <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
+  </numFmts>
+  <fonts count="23">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
       <name val="宋体"/>
       <charset val="134"/>
       <scheme val="minor"/>
@@ -144,14 +181,7 @@
       <sz val="12"/>
       <color rgb="FF24292F"/>
       <name val="Segoe UI"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="宋体"/>
       <charset val="134"/>
-      <scheme val="minor"/>
     </font>
     <font>
       <sz val="12"/>
@@ -161,7 +191,52 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF9C0006"/>
+      <color rgb="FFFF0000"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
       <name val="宋体"/>
       <charset val="134"/>
       <scheme val="minor"/>
@@ -170,46 +245,89 @@
       <sz val="11"/>
       <color rgb="FFFF0000"/>
       <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="宋体"/>
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <i/>
       <sz val="11"/>
-      <color rgb="FF9C0006"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
       <name val="宋体"/>
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="9"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
+      <color rgb="FF3F3F3F"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="宋体"/>
-      <family val="3"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="9"/>
-      <name val="宋体"/>
-      <family val="3"/>
-      <charset val="134"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="宋体"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="7">
+  <fills count="36">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -218,6 +336,18 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFD9FBD3"/>
         <bgColor indexed="64"/>
       </patternFill>
@@ -236,18 +366,180 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="10">
     <border>
       <left/>
       <right/>
@@ -270,15 +562,251 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="3">
+  <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="8" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="3" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="15" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="15" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="16" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -286,62 +814,104 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="31" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="7" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="3" fontId="1" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="31" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="7" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="3" fontId="3" fillId="6" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="1" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="4" fillId="6" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1">
-      <alignment vertical="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="31" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="7" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
-  <cellStyles count="3">
-    <cellStyle name="差" xfId="1" builtinId="27"/>
+  <cellStyles count="49">
     <cellStyle name="常规" xfId="0" builtinId="0"/>
-    <cellStyle name="好" xfId="2" builtinId="26"/>
+    <cellStyle name="货币[0]" xfId="1" builtinId="7"/>
+    <cellStyle name="20% - 强调文字颜色 3" xfId="2" builtinId="38"/>
+    <cellStyle name="输入" xfId="3" builtinId="20"/>
+    <cellStyle name="货币" xfId="4" builtinId="4"/>
+    <cellStyle name="千位分隔[0]" xfId="5" builtinId="6"/>
+    <cellStyle name="40% - 强调文字颜色 3" xfId="6" builtinId="39"/>
+    <cellStyle name="差" xfId="7" builtinId="27"/>
+    <cellStyle name="千位分隔" xfId="8" builtinId="3"/>
+    <cellStyle name="60% - 强调文字颜色 3" xfId="9" builtinId="40"/>
+    <cellStyle name="超链接" xfId="10" builtinId="8"/>
+    <cellStyle name="百分比" xfId="11" builtinId="5"/>
+    <cellStyle name="已访问的超链接" xfId="12" builtinId="9"/>
+    <cellStyle name="注释" xfId="13" builtinId="10"/>
+    <cellStyle name="60% - 强调文字颜色 2" xfId="14" builtinId="36"/>
+    <cellStyle name="标题 4" xfId="15" builtinId="19"/>
+    <cellStyle name="警告文本" xfId="16" builtinId="11"/>
+    <cellStyle name="标题" xfId="17" builtinId="15"/>
+    <cellStyle name="解释性文本" xfId="18" builtinId="53"/>
+    <cellStyle name="标题 1" xfId="19" builtinId="16"/>
+    <cellStyle name="标题 2" xfId="20" builtinId="17"/>
+    <cellStyle name="60% - 强调文字颜色 1" xfId="21" builtinId="32"/>
+    <cellStyle name="标题 3" xfId="22" builtinId="18"/>
+    <cellStyle name="60% - 强调文字颜色 4" xfId="23" builtinId="44"/>
+    <cellStyle name="输出" xfId="24" builtinId="21"/>
+    <cellStyle name="计算" xfId="25" builtinId="22"/>
+    <cellStyle name="检查单元格" xfId="26" builtinId="23"/>
+    <cellStyle name="20% - 强调文字颜色 6" xfId="27" builtinId="50"/>
+    <cellStyle name="强调文字颜色 2" xfId="28" builtinId="33"/>
+    <cellStyle name="链接单元格" xfId="29" builtinId="24"/>
+    <cellStyle name="汇总" xfId="30" builtinId="25"/>
+    <cellStyle name="好" xfId="31" builtinId="26"/>
+    <cellStyle name="适中" xfId="32" builtinId="28"/>
+    <cellStyle name="20% - 强调文字颜色 5" xfId="33" builtinId="46"/>
+    <cellStyle name="强调文字颜色 1" xfId="34" builtinId="29"/>
+    <cellStyle name="20% - 强调文字颜色 1" xfId="35" builtinId="30"/>
+    <cellStyle name="40% - 强调文字颜色 1" xfId="36" builtinId="31"/>
+    <cellStyle name="20% - 强调文字颜色 2" xfId="37" builtinId="34"/>
+    <cellStyle name="40% - 强调文字颜色 2" xfId="38" builtinId="35"/>
+    <cellStyle name="强调文字颜色 3" xfId="39" builtinId="37"/>
+    <cellStyle name="强调文字颜色 4" xfId="40" builtinId="41"/>
+    <cellStyle name="20% - 强调文字颜色 4" xfId="41" builtinId="42"/>
+    <cellStyle name="40% - 强调文字颜色 4" xfId="42" builtinId="43"/>
+    <cellStyle name="强调文字颜色 5" xfId="43" builtinId="45"/>
+    <cellStyle name="40% - 强调文字颜色 5" xfId="44" builtinId="47"/>
+    <cellStyle name="60% - 强调文字颜色 5" xfId="45" builtinId="48"/>
+    <cellStyle name="强调文字颜色 6" xfId="46" builtinId="49"/>
+    <cellStyle name="40% - 强调文字颜色 6" xfId="47" builtinId="51"/>
+    <cellStyle name="60% - 强调文字颜色 6" xfId="48" builtinId="52"/>
   </cellStyles>
-  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -628,98 +1198,98 @@
     </a:fmtScheme>
   </a:themeElements>
   <a:objectDefaults/>
-  <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
   <dimension ref="A1:F10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G10" sqref="G10"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1:F10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="24" customHeight="1" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="24" customHeight="1" outlineLevelCol="5"/>
   <cols>
     <col min="1" max="1" width="20" customWidth="1"/>
-    <col min="2" max="4" width="15.86328125" customWidth="1"/>
-    <col min="5" max="5" width="29.46484375" customWidth="1"/>
-    <col min="6" max="6" width="44.1328125" customWidth="1"/>
-    <col min="7" max="7" width="27.3984375" customWidth="1"/>
+    <col min="2" max="4" width="15.8666666666667" customWidth="1"/>
+    <col min="5" max="5" width="29.4666666666667" customWidth="1"/>
+    <col min="6" max="6" width="44.1333333333333" customWidth="1"/>
+    <col min="7" max="7" width="27.4" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="24" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="14" t="s">
+    <row r="1" customHeight="1" spans="1:6">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="14" t="s">
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="14" t="s">
+      <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="14" t="s">
+      <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="14" t="s">
+      <c r="E1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="14" t="s">
+      <c r="F1" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="24" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="14" t="s">
+    <row r="2" customHeight="1" spans="1:6">
+      <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="14"/>
-      <c r="C2" s="14"/>
-      <c r="D2" s="14"/>
-      <c r="E2" s="14"/>
-      <c r="F2" s="14"/>
-    </row>
-    <row r="3" spans="1:6" ht="24" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="16" t="s">
+      <c r="B2" s="1"/>
+      <c r="C2" s="1"/>
+      <c r="D2" s="1"/>
+      <c r="E2" s="1"/>
+      <c r="F2" s="1"/>
+    </row>
+    <row r="3" customHeight="1" spans="1:6">
+      <c r="A3" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="B3" s="16" t="s">
+      <c r="B3" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="C3" s="16" t="s">
+      <c r="C3" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="D3" s="16" t="s">
+      <c r="D3" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="E3" s="16" t="s">
+      <c r="E3" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="F3" s="16" t="s">
+      <c r="F3" s="2" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="4" spans="1:6" ht="24" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="14" t="s">
+    <row r="4" customHeight="1" spans="1:6">
+      <c r="A4" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="B4" s="14" t="s">
+      <c r="B4" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="C4" s="14" t="s">
+      <c r="C4" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="D4" s="14" t="s">
+      <c r="D4" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="E4" s="14" t="s">
+      <c r="E4" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="F4" s="14" t="s">
+      <c r="F4" s="1" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="5" spans="1:6" ht="24" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="5" customHeight="1" spans="2:6">
       <c r="B5">
         <v>100</v>
       </c>
@@ -736,7 +1306,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:6" ht="24" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="6" customHeight="1" spans="2:6">
       <c r="B6">
         <v>101</v>
       </c>
@@ -753,7 +1323,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:6" ht="24" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="7" customHeight="1" spans="2:6">
       <c r="B7">
         <v>102</v>
       </c>
@@ -770,7 +1340,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:6" ht="24" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="8" customHeight="1" spans="2:6">
       <c r="B8">
         <v>1000</v>
       </c>
@@ -787,7 +1357,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:6" ht="24" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="9" customHeight="1" spans="2:6">
       <c r="B9">
         <v>1001</v>
       </c>
@@ -804,15 +1374,15 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:6" ht="24" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="10" customHeight="1" spans="2:6">
       <c r="B10">
         <v>1002</v>
       </c>
-      <c r="C10" s="18" t="s">
-        <v>32</v>
-      </c>
-      <c r="D10" s="18" t="s">
-        <v>33</v>
+      <c r="C10" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="D10" s="3" t="s">
+        <v>17</v>
       </c>
       <c r="E10" t="b">
         <v>0</v>
@@ -822,326 +1392,434 @@
       </c>
     </row>
   </sheetData>
-  <phoneticPr fontId="8" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait"/>
+  <headerFooter/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
   <dimension ref="A1:F7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="16.86328125" defaultRowHeight="28.05" customHeight="1" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="16.8666666666667" defaultRowHeight="28.05" customHeight="1" outlineLevelRow="6" outlineLevelCol="5"/>
   <cols>
-    <col min="1" max="4" width="16.86328125" customWidth="1"/>
-    <col min="5" max="5" width="26.86328125" customWidth="1"/>
-    <col min="6" max="6" width="25.3984375" customWidth="1"/>
-    <col min="7" max="7" width="16.86328125" customWidth="1"/>
+    <col min="1" max="4" width="16.8666666666667" customWidth="1"/>
+    <col min="5" max="5" width="26.8666666666667" customWidth="1"/>
+    <col min="6" max="6" width="25.4" customWidth="1"/>
+    <col min="7" max="7" width="16.8666666666667" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="28.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="14" t="s">
+    <row r="1" customHeight="1" spans="1:6">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="14" t="s">
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="14" t="s">
+      <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="15"/>
-      <c r="E1" s="15"/>
-      <c r="F1" s="15"/>
-    </row>
-    <row r="2" spans="1:6" ht="28.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="14" t="s">
+      <c r="D1" s="17"/>
+      <c r="E1" s="17"/>
+      <c r="F1" s="17"/>
+    </row>
+    <row r="2" customHeight="1" spans="1:6">
+      <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="14"/>
-      <c r="C2" s="14"/>
-      <c r="D2" s="15"/>
-      <c r="E2" s="15"/>
-      <c r="F2" s="15"/>
-    </row>
-    <row r="3" spans="1:6" ht="28.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="16" t="s">
+      <c r="B2" s="1"/>
+      <c r="C2" s="1"/>
+      <c r="D2" s="17"/>
+      <c r="E2" s="17"/>
+      <c r="F2" s="17"/>
+    </row>
+    <row r="3" customHeight="1" spans="1:6">
+      <c r="A3" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="B3" s="16" t="s">
+      <c r="B3" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="C3" s="16" t="s">
+      <c r="C3" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="D3" s="17"/>
-      <c r="E3" s="17"/>
-      <c r="F3" s="17"/>
-    </row>
-    <row r="4" spans="1:6" ht="28.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="14" t="s">
+      <c r="D3" s="18"/>
+      <c r="E3" s="18"/>
+      <c r="F3" s="18"/>
+    </row>
+    <row r="4" customHeight="1" spans="1:6">
+      <c r="A4" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="B4" s="14" t="s">
-        <v>22</v>
-      </c>
-      <c r="C4" s="14" t="s">
+      <c r="B4" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C4" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="D4" s="15"/>
-      <c r="E4" s="15"/>
-      <c r="F4" s="15"/>
-    </row>
-    <row r="5" spans="1:6" ht="28.05" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="D4" s="17"/>
+      <c r="E4" s="17"/>
+      <c r="F4" s="17"/>
+    </row>
+    <row r="5" customHeight="1" spans="2:3">
       <c r="B5">
         <v>10000</v>
       </c>
       <c r="C5" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" ht="28.05" customHeight="1" x14ac:dyDescent="0.3">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="6" customHeight="1" spans="2:3">
       <c r="B6">
         <v>10001</v>
       </c>
       <c r="C6" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" ht="28.05" customHeight="1" x14ac:dyDescent="0.3">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="7" customHeight="1" spans="2:3">
       <c r="B7">
         <v>10002</v>
       </c>
       <c r="C7" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
     </row>
   </sheetData>
-  <phoneticPr fontId="10" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait"/>
+  <headerFooter/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
   <dimension ref="A1:F25"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="24" customHeight="1" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="24" customHeight="1" outlineLevelCol="5"/>
   <cols>
-    <col min="1" max="1" width="20" style="1" customWidth="1"/>
-    <col min="2" max="2" width="15.86328125" style="2" customWidth="1"/>
-    <col min="3" max="3" width="19.73046875" style="3" customWidth="1"/>
-    <col min="4" max="4" width="15.86328125" style="3" customWidth="1"/>
-    <col min="5" max="5" width="29.46484375" customWidth="1"/>
-    <col min="6" max="6" width="44.1328125" customWidth="1"/>
-    <col min="7" max="7" width="27.3984375" customWidth="1"/>
+    <col min="1" max="1" width="20" style="4" customWidth="1"/>
+    <col min="2" max="2" width="15.8666666666667" style="5" customWidth="1"/>
+    <col min="3" max="3" width="19.7333333333333" style="6" customWidth="1"/>
+    <col min="4" max="4" width="15.8666666666667" style="6" customWidth="1"/>
+    <col min="5" max="5" width="29.4666666666667" customWidth="1"/>
+    <col min="6" max="6" width="44.1333333333333" customWidth="1"/>
+    <col min="7" max="7" width="27.4" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="24" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="B1" s="5" t="s">
+    <row r="1" customHeight="1" spans="1:6">
+      <c r="A1" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="B1" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="C1" s="6" t="s">
+      <c r="C1" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="D1" s="6"/>
-      <c r="E1" s="7"/>
-      <c r="F1" s="7"/>
-    </row>
-    <row r="2" spans="1:6" ht="24" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="4" t="s">
-        <v>27</v>
-      </c>
-      <c r="B2" s="5" t="s">
+      <c r="D1" s="9"/>
+      <c r="E1" s="10"/>
+      <c r="F1" s="10"/>
+    </row>
+    <row r="2" customHeight="1" spans="1:6">
+      <c r="A2" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="B2" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="C2" s="8"/>
-      <c r="D2" s="6" t="b">
+      <c r="C2" s="11"/>
+      <c r="D2" s="9" t="b">
         <v>0</v>
       </c>
-      <c r="E2" s="7"/>
-      <c r="F2" s="7"/>
-    </row>
-    <row r="3" spans="1:6" ht="24" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="B3" s="5" t="s">
+      <c r="E2" s="10"/>
+      <c r="F2" s="10"/>
+    </row>
+    <row r="3" customHeight="1" spans="1:6">
+      <c r="A3" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="B3" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="C3" s="8"/>
-      <c r="D3" s="6" t="b">
+      <c r="C3" s="11"/>
+      <c r="D3" s="9" t="b">
         <v>0</v>
       </c>
-      <c r="E3" s="9"/>
-      <c r="F3" s="9"/>
-    </row>
-    <row r="4" spans="1:6" ht="24" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="4" t="s">
-        <v>29</v>
-      </c>
-      <c r="B4" s="5" t="s">
+      <c r="E3" s="12"/>
+      <c r="F3" s="12"/>
+    </row>
+    <row r="4" customHeight="1" spans="1:6">
+      <c r="A4" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="B4" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="C4" s="8"/>
-      <c r="D4" s="6">
+      <c r="C4" s="11"/>
+      <c r="D4" s="9">
         <v>1</v>
       </c>
-      <c r="E4" s="7"/>
-      <c r="F4" s="7"/>
-    </row>
-    <row r="5" spans="1:6" ht="24" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="4" t="s">
-        <v>30</v>
-      </c>
-      <c r="B5" s="5" t="s">
+      <c r="E4" s="10"/>
+      <c r="F4" s="10"/>
+    </row>
+    <row r="5" customHeight="1" spans="1:4">
+      <c r="A5" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="B5" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="C5" s="8"/>
-      <c r="D5" s="10">
+      <c r="C5" s="11"/>
+      <c r="D5" s="13">
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:6" ht="24" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="4" t="s">
-        <v>31</v>
-      </c>
-      <c r="B6" s="5" t="s">
+    <row r="6" customHeight="1" spans="1:4">
+      <c r="A6" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="B6" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="C6" s="11"/>
-      <c r="D6" s="10">
+      <c r="C6" s="14"/>
+      <c r="D6" s="13">
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:6" ht="24" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="12"/>
-      <c r="B7" s="13"/>
-      <c r="C7" s="11"/>
-      <c r="D7" s="11"/>
-    </row>
-    <row r="8" spans="1:6" ht="24" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="12"/>
-      <c r="B8" s="13"/>
-      <c r="C8" s="11"/>
-      <c r="D8" s="11"/>
-    </row>
-    <row r="9" spans="1:6" ht="24" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="12"/>
-      <c r="B9" s="13"/>
-      <c r="C9" s="11"/>
-      <c r="D9" s="11"/>
-    </row>
-    <row r="10" spans="1:6" ht="24" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="12"/>
-      <c r="B10" s="13"/>
-      <c r="C10" s="11"/>
-      <c r="D10" s="11"/>
-    </row>
-    <row r="11" spans="1:6" ht="24" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="12"/>
-      <c r="B11" s="13"/>
-      <c r="C11" s="11"/>
-      <c r="D11" s="11"/>
-    </row>
-    <row r="12" spans="1:6" ht="24" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="12"/>
-      <c r="B12" s="13"/>
-      <c r="C12" s="11"/>
-      <c r="D12" s="11"/>
-    </row>
-    <row r="13" spans="1:6" ht="24" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="12"/>
-      <c r="B13" s="13"/>
-      <c r="C13" s="11"/>
-      <c r="D13" s="11"/>
-    </row>
-    <row r="14" spans="1:6" ht="24" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="12"/>
-      <c r="B14" s="13"/>
-      <c r="C14" s="11"/>
-      <c r="D14" s="11"/>
-    </row>
-    <row r="15" spans="1:6" ht="24" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="12"/>
-      <c r="B15" s="13"/>
-      <c r="C15" s="11"/>
-      <c r="D15" s="11"/>
-    </row>
-    <row r="16" spans="1:6" ht="24" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="12"/>
-      <c r="B16" s="13"/>
-      <c r="C16" s="11"/>
-      <c r="D16" s="11"/>
-    </row>
-    <row r="17" spans="1:4" ht="24" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="12"/>
-      <c r="B17" s="13"/>
-      <c r="C17" s="11"/>
-      <c r="D17" s="11"/>
-    </row>
-    <row r="18" spans="1:4" ht="24" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="12"/>
-      <c r="B18" s="13"/>
-      <c r="C18" s="11"/>
-      <c r="D18" s="11"/>
-    </row>
-    <row r="19" spans="1:4" ht="24" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="12"/>
-      <c r="B19" s="13"/>
-      <c r="C19" s="11"/>
-      <c r="D19" s="11"/>
-    </row>
-    <row r="20" spans="1:4" ht="24" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="12"/>
-      <c r="B20" s="13"/>
-      <c r="C20" s="11"/>
-      <c r="D20" s="11"/>
-    </row>
-    <row r="21" spans="1:4" ht="24" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="12"/>
-      <c r="B21" s="13"/>
-      <c r="C21" s="11"/>
-      <c r="D21" s="11"/>
-    </row>
-    <row r="22" spans="1:4" ht="24" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="12"/>
-      <c r="B22" s="13"/>
-      <c r="C22" s="11"/>
-      <c r="D22" s="11"/>
-    </row>
-    <row r="23" spans="1:4" ht="24" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A23" s="12"/>
-      <c r="B23" s="13"/>
-      <c r="C23" s="11"/>
-      <c r="D23" s="11"/>
-    </row>
-    <row r="24" spans="1:4" ht="24" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A24" s="12"/>
-      <c r="B24" s="13"/>
-      <c r="C24" s="11"/>
-      <c r="D24" s="11"/>
-    </row>
-    <row r="25" spans="1:4" ht="24" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A25" s="12"/>
-      <c r="B25" s="13"/>
-      <c r="C25" s="11"/>
-      <c r="D25" s="11"/>
+    <row r="7" customHeight="1" spans="1:4">
+      <c r="A7" s="15"/>
+      <c r="B7" s="16"/>
+      <c r="C7" s="14"/>
+      <c r="D7" s="14"/>
+    </row>
+    <row r="8" customHeight="1" spans="1:4">
+      <c r="A8" s="15"/>
+      <c r="B8" s="16"/>
+      <c r="C8" s="14"/>
+      <c r="D8" s="14"/>
+    </row>
+    <row r="9" customHeight="1" spans="1:4">
+      <c r="A9" s="15"/>
+      <c r="B9" s="16"/>
+      <c r="C9" s="14"/>
+      <c r="D9" s="14"/>
+    </row>
+    <row r="10" customHeight="1" spans="1:4">
+      <c r="A10" s="15"/>
+      <c r="B10" s="16"/>
+      <c r="C10" s="14"/>
+      <c r="D10" s="14"/>
+    </row>
+    <row r="11" customHeight="1" spans="1:4">
+      <c r="A11" s="15"/>
+      <c r="B11" s="16"/>
+      <c r="C11" s="14"/>
+      <c r="D11" s="14"/>
+    </row>
+    <row r="12" customHeight="1" spans="1:4">
+      <c r="A12" s="15"/>
+      <c r="B12" s="16"/>
+      <c r="C12" s="14"/>
+      <c r="D12" s="14"/>
+    </row>
+    <row r="13" customHeight="1" spans="1:4">
+      <c r="A13" s="15"/>
+      <c r="B13" s="16"/>
+      <c r="C13" s="14"/>
+      <c r="D13" s="14"/>
+    </row>
+    <row r="14" customHeight="1" spans="1:4">
+      <c r="A14" s="15"/>
+      <c r="B14" s="16"/>
+      <c r="C14" s="14"/>
+      <c r="D14" s="14"/>
+    </row>
+    <row r="15" customHeight="1" spans="1:4">
+      <c r="A15" s="15"/>
+      <c r="B15" s="16"/>
+      <c r="C15" s="14"/>
+      <c r="D15" s="14"/>
+    </row>
+    <row r="16" customHeight="1" spans="1:4">
+      <c r="A16" s="15"/>
+      <c r="B16" s="16"/>
+      <c r="C16" s="14"/>
+      <c r="D16" s="14"/>
+    </row>
+    <row r="17" customHeight="1" spans="1:4">
+      <c r="A17" s="15"/>
+      <c r="B17" s="16"/>
+      <c r="C17" s="14"/>
+      <c r="D17" s="14"/>
+    </row>
+    <row r="18" customHeight="1" spans="1:4">
+      <c r="A18" s="15"/>
+      <c r="B18" s="16"/>
+      <c r="C18" s="14"/>
+      <c r="D18" s="14"/>
+    </row>
+    <row r="19" customHeight="1" spans="1:4">
+      <c r="A19" s="15"/>
+      <c r="B19" s="16"/>
+      <c r="C19" s="14"/>
+      <c r="D19" s="14"/>
+    </row>
+    <row r="20" customHeight="1" spans="1:4">
+      <c r="A20" s="15"/>
+      <c r="B20" s="16"/>
+      <c r="C20" s="14"/>
+      <c r="D20" s="14"/>
+    </row>
+    <row r="21" customHeight="1" spans="1:4">
+      <c r="A21" s="15"/>
+      <c r="B21" s="16"/>
+      <c r="C21" s="14"/>
+      <c r="D21" s="14"/>
+    </row>
+    <row r="22" customHeight="1" spans="1:4">
+      <c r="A22" s="15"/>
+      <c r="B22" s="16"/>
+      <c r="C22" s="14"/>
+      <c r="D22" s="14"/>
+    </row>
+    <row r="23" customHeight="1" spans="1:4">
+      <c r="A23" s="15"/>
+      <c r="B23" s="16"/>
+      <c r="C23" s="14"/>
+      <c r="D23" s="14"/>
+    </row>
+    <row r="24" customHeight="1" spans="1:4">
+      <c r="A24" s="15"/>
+      <c r="B24" s="16"/>
+      <c r="C24" s="14"/>
+      <c r="D24" s="14"/>
+    </row>
+    <row r="25" customHeight="1" spans="1:4">
+      <c r="A25" s="15"/>
+      <c r="B25" s="16"/>
+      <c r="C25" s="14"/>
+      <c r="D25" s="14"/>
     </row>
   </sheetData>
-  <phoneticPr fontId="10" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <headerFooter/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
+  <dimension ref="A1:C10"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F7" sqref="F7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="25" defaultRowHeight="27" customHeight="1" outlineLevelCol="2"/>
+  <cols>
+    <col min="1" max="2" width="25" customWidth="1"/>
+    <col min="3" max="3" width="26.375" customWidth="1"/>
+    <col min="4" max="16381" width="25" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" customHeight="1" spans="1:3">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="2" customHeight="1" spans="1:3">
+      <c r="A2" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="1"/>
+      <c r="C2" s="1"/>
+    </row>
+    <row r="3" customHeight="1" spans="1:3">
+      <c r="A3" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="4" customHeight="1" spans="1:3">
+      <c r="A4" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="5" customHeight="1" spans="2:3">
+      <c r="B5" t="s">
+        <v>37</v>
+      </c>
+      <c r="C5" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" customHeight="1" spans="2:3">
+      <c r="B6" t="s">
+        <v>38</v>
+      </c>
+      <c r="C6" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" customHeight="1" spans="2:3">
+      <c r="B7" t="s">
+        <v>39</v>
+      </c>
+      <c r="C7" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" customHeight="1" spans="2:3">
+      <c r="B8" t="s">
+        <v>40</v>
+      </c>
+      <c r="C8" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" customHeight="1" spans="2:3">
+      <c r="B9" t="s">
+        <v>41</v>
+      </c>
+      <c r="C9" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" customHeight="1" spans="2:3">
+      <c r="B10" s="3"/>
+      <c r="C10" s="3"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <headerFooter/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
update change scene by select
</commit_message>
<xml_diff>
--- a/Luban/Config/Datas/Config.xlsx
+++ b/Luban/Config/Datas/Config.xlsx
@@ -1,28 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="25601"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\GameDev\Blues-Dusk\Luban\Config\Datas\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A2E255CA-7655-4303-A967-1DD546EA53B8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-22728" yWindow="6312" windowWidth="17280" windowHeight="8808" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView windowWidth="28125" windowHeight="12540" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="UIConfig" sheetId="1" r:id="rId1"/>
     <sheet name="EntityConfig" sheetId="2" r:id="rId2"/>
     <sheet name="GameConfig" sheetId="3" r:id="rId3"/>
+    <sheet name="SceneConfig" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="144525"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="46">
   <si>
     <t>##var</t>
   </si>
@@ -90,6 +85,21 @@
     <t>UI_Backpack</t>
   </si>
   <si>
+    <t>UI_GameMenu</t>
+  </si>
+  <si>
+    <t>UI_DiceInventory</t>
+  </si>
+  <si>
+    <t>UI_Tip</t>
+  </si>
+  <si>
+    <t>General</t>
+  </si>
+  <si>
+    <t>UI_SelectScene</t>
+  </si>
+  <si>
     <t>实体编号</t>
   </si>
   <si>
@@ -120,23 +130,65 @@
     <t>current_week</t>
   </si>
   <si>
-    <t>UI_GameMenu</t>
-    <phoneticPr fontId="8" type="noConversion"/>
-  </si>
-  <si>
-    <t>Default</t>
-    <phoneticPr fontId="8" type="noConversion"/>
-  </si>
-  <si>
-    <t>UI_DiceInventory</t>
-    <phoneticPr fontId="8" type="noConversion"/>
+    <t>scene_asset_name</t>
+  </si>
+  <si>
+    <t>is_unlocked</t>
+  </si>
+  <si>
+    <t>场景资源名</t>
+  </si>
+  <si>
+    <t>是否解锁</t>
+  </si>
+  <si>
+    <t>S_Parlor</t>
+  </si>
+  <si>
+    <t>S_Station</t>
+  </si>
+  <si>
+    <t>S_Bar</t>
+  </si>
+  <si>
+    <t>S_FengHospital</t>
+  </si>
+  <si>
+    <t>S_Tower</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="11" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <numFmts count="4">
+    <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
+  </numFmts>
+  <fonts count="24">
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -148,14 +200,7 @@
       <sz val="12"/>
       <color rgb="FF24292F"/>
       <name val="Segoe UI"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="宋体"/>
       <charset val="134"/>
-      <scheme val="minor"/>
     </font>
     <font>
       <sz val="12"/>
@@ -165,7 +210,52 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF9C0006"/>
+      <color rgb="FFFF0000"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
       <name val="宋体"/>
       <charset val="134"/>
       <scheme val="minor"/>
@@ -174,46 +264,89 @@
       <sz val="11"/>
       <color rgb="FFFF0000"/>
       <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="宋体"/>
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <i/>
       <sz val="11"/>
-      <color rgb="FF9C0006"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
       <name val="宋体"/>
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="9"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
+      <color rgb="FF3F3F3F"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="宋体"/>
-      <family val="3"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="9"/>
-      <name val="宋体"/>
-      <family val="3"/>
-      <charset val="134"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="宋体"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="7">
+  <fills count="36">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -222,6 +355,18 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFD9FBD3"/>
         <bgColor indexed="64"/>
       </patternFill>
@@ -240,18 +385,180 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="10">
     <border>
       <left/>
       <right/>
@@ -274,15 +581,251 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="3">
+  <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="8" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="3" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="15" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="15" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="16" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -290,62 +833,104 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="31" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="7" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="31" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="3" fontId="1" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="7" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="3" fontId="4" fillId="6" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="1" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="4" fillId="6" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1">
-      <alignment vertical="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="31" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="7" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
-  <cellStyles count="3">
-    <cellStyle name="差" xfId="1" builtinId="27"/>
+  <cellStyles count="49">
     <cellStyle name="常规" xfId="0" builtinId="0"/>
-    <cellStyle name="好" xfId="2" builtinId="26"/>
+    <cellStyle name="货币[0]" xfId="1" builtinId="7"/>
+    <cellStyle name="20% - 强调文字颜色 3" xfId="2" builtinId="38"/>
+    <cellStyle name="输入" xfId="3" builtinId="20"/>
+    <cellStyle name="货币" xfId="4" builtinId="4"/>
+    <cellStyle name="千位分隔[0]" xfId="5" builtinId="6"/>
+    <cellStyle name="40% - 强调文字颜色 3" xfId="6" builtinId="39"/>
+    <cellStyle name="差" xfId="7" builtinId="27"/>
+    <cellStyle name="千位分隔" xfId="8" builtinId="3"/>
+    <cellStyle name="60% - 强调文字颜色 3" xfId="9" builtinId="40"/>
+    <cellStyle name="超链接" xfId="10" builtinId="8"/>
+    <cellStyle name="百分比" xfId="11" builtinId="5"/>
+    <cellStyle name="已访问的超链接" xfId="12" builtinId="9"/>
+    <cellStyle name="注释" xfId="13" builtinId="10"/>
+    <cellStyle name="60% - 强调文字颜色 2" xfId="14" builtinId="36"/>
+    <cellStyle name="标题 4" xfId="15" builtinId="19"/>
+    <cellStyle name="警告文本" xfId="16" builtinId="11"/>
+    <cellStyle name="标题" xfId="17" builtinId="15"/>
+    <cellStyle name="解释性文本" xfId="18" builtinId="53"/>
+    <cellStyle name="标题 1" xfId="19" builtinId="16"/>
+    <cellStyle name="标题 2" xfId="20" builtinId="17"/>
+    <cellStyle name="60% - 强调文字颜色 1" xfId="21" builtinId="32"/>
+    <cellStyle name="标题 3" xfId="22" builtinId="18"/>
+    <cellStyle name="60% - 强调文字颜色 4" xfId="23" builtinId="44"/>
+    <cellStyle name="输出" xfId="24" builtinId="21"/>
+    <cellStyle name="计算" xfId="25" builtinId="22"/>
+    <cellStyle name="检查单元格" xfId="26" builtinId="23"/>
+    <cellStyle name="20% - 强调文字颜色 6" xfId="27" builtinId="50"/>
+    <cellStyle name="强调文字颜色 2" xfId="28" builtinId="33"/>
+    <cellStyle name="链接单元格" xfId="29" builtinId="24"/>
+    <cellStyle name="汇总" xfId="30" builtinId="25"/>
+    <cellStyle name="好" xfId="31" builtinId="26"/>
+    <cellStyle name="适中" xfId="32" builtinId="28"/>
+    <cellStyle name="20% - 强调文字颜色 5" xfId="33" builtinId="46"/>
+    <cellStyle name="强调文字颜色 1" xfId="34" builtinId="29"/>
+    <cellStyle name="20% - 强调文字颜色 1" xfId="35" builtinId="30"/>
+    <cellStyle name="40% - 强调文字颜色 1" xfId="36" builtinId="31"/>
+    <cellStyle name="20% - 强调文字颜色 2" xfId="37" builtinId="34"/>
+    <cellStyle name="40% - 强调文字颜色 2" xfId="38" builtinId="35"/>
+    <cellStyle name="强调文字颜色 3" xfId="39" builtinId="37"/>
+    <cellStyle name="强调文字颜色 4" xfId="40" builtinId="41"/>
+    <cellStyle name="20% - 强调文字颜色 4" xfId="41" builtinId="42"/>
+    <cellStyle name="40% - 强调文字颜色 4" xfId="42" builtinId="43"/>
+    <cellStyle name="强调文字颜色 5" xfId="43" builtinId="45"/>
+    <cellStyle name="40% - 强调文字颜色 5" xfId="44" builtinId="47"/>
+    <cellStyle name="60% - 强调文字颜色 5" xfId="45" builtinId="48"/>
+    <cellStyle name="强调文字颜色 6" xfId="46" builtinId="49"/>
+    <cellStyle name="40% - 强调文字颜色 6" xfId="47" builtinId="51"/>
+    <cellStyle name="60% - 强调文字颜色 6" xfId="48" builtinId="52"/>
   </cellStyles>
-  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -632,98 +1217,98 @@
     </a:fmtScheme>
   </a:themeElements>
   <a:objectDefaults/>
-  <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F11"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
+  <dimension ref="A1:F13"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="E12" sqref="E12"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1:D13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="24" customHeight="1" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="24" customHeight="1" outlineLevelCol="5"/>
   <cols>
     <col min="1" max="1" width="20" customWidth="1"/>
-    <col min="2" max="4" width="15.86328125" customWidth="1"/>
-    <col min="5" max="5" width="29.46484375" customWidth="1"/>
-    <col min="6" max="6" width="44.1328125" customWidth="1"/>
-    <col min="7" max="7" width="27.3984375" customWidth="1"/>
+    <col min="2" max="4" width="15.8666666666667" customWidth="1"/>
+    <col min="5" max="5" width="29.4666666666667" customWidth="1"/>
+    <col min="6" max="6" width="44.1333333333333" customWidth="1"/>
+    <col min="7" max="7" width="27.4" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="24" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="14" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="14" t="s">
+    <row r="1" customHeight="1" spans="1:6">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="14" t="s">
+      <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="14" t="s">
+      <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="14" t="s">
+      <c r="E1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="14" t="s">
+      <c r="F1" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="24" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="14" t="s">
-        <v>0</v>
-      </c>
-      <c r="B2" s="14"/>
-      <c r="C2" s="14"/>
-      <c r="D2" s="14"/>
-      <c r="E2" s="14"/>
-      <c r="F2" s="14"/>
-    </row>
-    <row r="3" spans="1:6" ht="24" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="16" t="s">
+    <row r="2" customHeight="1" spans="1:6">
+      <c r="A2" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="1"/>
+      <c r="C2" s="1"/>
+      <c r="D2" s="1"/>
+      <c r="E2" s="1"/>
+      <c r="F2" s="1"/>
+    </row>
+    <row r="3" customHeight="1" spans="1:6">
+      <c r="A3" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="B3" s="16" t="s">
+      <c r="B3" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="C3" s="16" t="s">
+      <c r="C3" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="D3" s="16" t="s">
+      <c r="D3" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="E3" s="16" t="s">
+      <c r="E3" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="F3" s="16" t="s">
+      <c r="F3" s="2" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="4" spans="1:6" ht="24" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="14" t="s">
+    <row r="4" customHeight="1" spans="1:6">
+      <c r="A4" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="B4" s="14" t="s">
+      <c r="B4" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="C4" s="14" t="s">
+      <c r="C4" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="D4" s="14" t="s">
+      <c r="D4" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="E4" s="14" t="s">
+      <c r="E4" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="F4" s="14" t="s">
+      <c r="F4" s="1" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="5" spans="1:6" ht="24" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="5" customHeight="1" spans="2:6">
       <c r="B5">
         <v>100</v>
       </c>
@@ -740,7 +1325,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:6" ht="24" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="6" customHeight="1" spans="2:6">
       <c r="B6">
         <v>101</v>
       </c>
@@ -757,7 +1342,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:6" ht="24" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="7" customHeight="1" spans="2:6">
       <c r="B7">
         <v>102</v>
       </c>
@@ -774,7 +1359,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:6" ht="24" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="8" customHeight="1" spans="2:6">
       <c r="B8">
         <v>1000</v>
       </c>
@@ -791,7 +1376,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:6" ht="24" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="9" customHeight="1" spans="2:6">
       <c r="B9">
         <v>1001</v>
       </c>
@@ -805,18 +1390,18 @@
         <v>0</v>
       </c>
       <c r="F9" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" ht="24" customHeight="1" x14ac:dyDescent="0.3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" customHeight="1" spans="2:6">
       <c r="B10">
         <v>1002</v>
       </c>
-      <c r="C10" s="18" t="s">
-        <v>32</v>
-      </c>
-      <c r="D10" s="18" t="s">
-        <v>33</v>
+      <c r="C10" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="D10" s="3" t="s">
+        <v>17</v>
       </c>
       <c r="E10" t="b">
         <v>0</v>
@@ -825,344 +1410,488 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:6" ht="24" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="11" customHeight="1" spans="2:6">
       <c r="B11">
         <v>1003</v>
       </c>
-      <c r="C11" s="18" t="s">
-        <v>34</v>
-      </c>
-      <c r="D11" s="18" t="s">
-        <v>33</v>
-      </c>
-      <c r="E11" s="18" t="b">
+      <c r="C11" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="D11" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="E11" s="3" t="b">
         <v>0</v>
       </c>
       <c r="F11" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" customHeight="1" spans="2:6">
+      <c r="B12">
+        <v>1004</v>
+      </c>
+      <c r="C12" t="s">
+        <v>24</v>
+      </c>
+      <c r="D12" t="s">
+        <v>25</v>
+      </c>
+      <c r="E12" s="3" t="b">
+        <v>0</v>
+      </c>
+      <c r="F12" t="b">
         <v>1</v>
       </c>
     </row>
+    <row r="13" customHeight="1" spans="2:6">
+      <c r="B13">
+        <v>1005</v>
+      </c>
+      <c r="C13" t="s">
+        <v>26</v>
+      </c>
+      <c r="D13" t="s">
+        <v>25</v>
+      </c>
+      <c r="E13" s="3" t="b">
+        <v>0</v>
+      </c>
+      <c r="F13" t="b">
+        <v>1</v>
+      </c>
+    </row>
   </sheetData>
-  <phoneticPr fontId="8" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait"/>
+  <headerFooter/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
   <dimension ref="A1:F7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="16.86328125" defaultRowHeight="28.05" customHeight="1" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="16.8666666666667" defaultRowHeight="28.05" customHeight="1" outlineLevelRow="6" outlineLevelCol="5"/>
   <cols>
-    <col min="1" max="4" width="16.86328125" customWidth="1"/>
-    <col min="5" max="5" width="26.86328125" customWidth="1"/>
-    <col min="6" max="6" width="25.3984375" customWidth="1"/>
-    <col min="7" max="7" width="16.86328125" customWidth="1"/>
+    <col min="1" max="4" width="16.8666666666667" customWidth="1"/>
+    <col min="5" max="5" width="26.8666666666667" customWidth="1"/>
+    <col min="6" max="6" width="25.4" customWidth="1"/>
+    <col min="7" max="7" width="16.8666666666667" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="28.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="14" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="14" t="s">
+    <row r="1" customHeight="1" spans="1:6">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="14" t="s">
+      <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="15"/>
-      <c r="E1" s="15"/>
-      <c r="F1" s="15"/>
-    </row>
-    <row r="2" spans="1:6" ht="28.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="14" t="s">
-        <v>0</v>
-      </c>
-      <c r="B2" s="14"/>
-      <c r="C2" s="14"/>
-      <c r="D2" s="15"/>
-      <c r="E2" s="15"/>
-      <c r="F2" s="15"/>
-    </row>
-    <row r="3" spans="1:6" ht="28.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="16" t="s">
+      <c r="D1" s="17"/>
+      <c r="E1" s="17"/>
+      <c r="F1" s="17"/>
+    </row>
+    <row r="2" customHeight="1" spans="1:6">
+      <c r="A2" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="1"/>
+      <c r="C2" s="1"/>
+      <c r="D2" s="17"/>
+      <c r="E2" s="17"/>
+      <c r="F2" s="17"/>
+    </row>
+    <row r="3" customHeight="1" spans="1:6">
+      <c r="A3" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="B3" s="16" t="s">
+      <c r="B3" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="C3" s="16" t="s">
+      <c r="C3" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="D3" s="17"/>
-      <c r="E3" s="17"/>
-      <c r="F3" s="17"/>
-    </row>
-    <row r="4" spans="1:6" ht="28.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="14" t="s">
+      <c r="D3" s="18"/>
+      <c r="E3" s="18"/>
+      <c r="F3" s="18"/>
+    </row>
+    <row r="4" customHeight="1" spans="1:6">
+      <c r="A4" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="B4" s="14" t="s">
-        <v>22</v>
-      </c>
-      <c r="C4" s="14" t="s">
+      <c r="B4" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="C4" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="D4" s="15"/>
-      <c r="E4" s="15"/>
-      <c r="F4" s="15"/>
-    </row>
-    <row r="5" spans="1:6" ht="28.05" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="D4" s="17"/>
+      <c r="E4" s="17"/>
+      <c r="F4" s="17"/>
+    </row>
+    <row r="5" customHeight="1" spans="2:3">
       <c r="B5">
         <v>10000</v>
       </c>
       <c r="C5" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" ht="28.05" customHeight="1" x14ac:dyDescent="0.3">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="6" customHeight="1" spans="2:3">
       <c r="B6">
         <v>10001</v>
       </c>
       <c r="C6" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" ht="28.05" customHeight="1" x14ac:dyDescent="0.3">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="7" customHeight="1" spans="2:3">
       <c r="B7">
         <v>10002</v>
       </c>
       <c r="C7" t="s">
-        <v>25</v>
+        <v>30</v>
       </c>
     </row>
   </sheetData>
-  <phoneticPr fontId="10" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait"/>
+  <headerFooter/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
   <dimension ref="A1:F25"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="24" customHeight="1" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="24" customHeight="1" outlineLevelCol="5"/>
   <cols>
-    <col min="1" max="1" width="20" style="1" customWidth="1"/>
-    <col min="2" max="2" width="15.86328125" style="2" customWidth="1"/>
-    <col min="3" max="3" width="19.73046875" style="3" customWidth="1"/>
-    <col min="4" max="4" width="15.86328125" style="3" customWidth="1"/>
-    <col min="5" max="5" width="29.46484375" customWidth="1"/>
-    <col min="6" max="6" width="44.1328125" customWidth="1"/>
-    <col min="7" max="7" width="27.3984375" customWidth="1"/>
+    <col min="1" max="1" width="20" style="4" customWidth="1"/>
+    <col min="2" max="2" width="15.8666666666667" style="5" customWidth="1"/>
+    <col min="3" max="3" width="19.7333333333333" style="6" customWidth="1"/>
+    <col min="4" max="4" width="15.8666666666667" style="6" customWidth="1"/>
+    <col min="5" max="5" width="29.4666666666667" customWidth="1"/>
+    <col min="6" max="6" width="44.1333333333333" customWidth="1"/>
+    <col min="7" max="7" width="27.4" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="24" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="B1" s="5" t="s">
+    <row r="1" customHeight="1" spans="1:6">
+      <c r="A1" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="B1" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="C1" s="6" t="s">
+      <c r="C1" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="D1" s="6"/>
-      <c r="E1" s="7"/>
-      <c r="F1" s="7"/>
-    </row>
-    <row r="2" spans="1:6" ht="24" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="4" t="s">
-        <v>27</v>
-      </c>
-      <c r="B2" s="5" t="s">
+      <c r="D1" s="9"/>
+      <c r="E1" s="10"/>
+      <c r="F1" s="10"/>
+    </row>
+    <row r="2" customHeight="1" spans="1:6">
+      <c r="A2" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="B2" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="C2" s="8"/>
-      <c r="D2" s="6" t="b">
-        <v>0</v>
-      </c>
-      <c r="E2" s="7"/>
-      <c r="F2" s="7"/>
-    </row>
-    <row r="3" spans="1:6" ht="24" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="B3" s="5" t="s">
+      <c r="C2" s="11"/>
+      <c r="D2" s="9" t="b">
+        <v>0</v>
+      </c>
+      <c r="E2" s="10"/>
+      <c r="F2" s="10"/>
+    </row>
+    <row r="3" customHeight="1" spans="1:6">
+      <c r="A3" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="B3" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="C3" s="8"/>
-      <c r="D3" s="6" t="b">
-        <v>0</v>
-      </c>
-      <c r="E3" s="9"/>
-      <c r="F3" s="9"/>
-    </row>
-    <row r="4" spans="1:6" ht="24" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="4" t="s">
-        <v>29</v>
-      </c>
-      <c r="B4" s="5" t="s">
+      <c r="C3" s="11"/>
+      <c r="D3" s="9" t="b">
+        <v>0</v>
+      </c>
+      <c r="E3" s="12"/>
+      <c r="F3" s="12"/>
+    </row>
+    <row r="4" customHeight="1" spans="1:6">
+      <c r="A4" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="B4" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="C4" s="8"/>
-      <c r="D4" s="6">
+      <c r="C4" s="11"/>
+      <c r="D4" s="9">
         <v>1</v>
       </c>
-      <c r="E4" s="7"/>
-      <c r="F4" s="7"/>
-    </row>
-    <row r="5" spans="1:6" ht="24" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="4" t="s">
-        <v>30</v>
-      </c>
-      <c r="B5" s="5" t="s">
+      <c r="E4" s="10"/>
+      <c r="F4" s="10"/>
+    </row>
+    <row r="5" customHeight="1" spans="1:4">
+      <c r="A5" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="B5" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="C5" s="8"/>
-      <c r="D5" s="10">
+      <c r="C5" s="11"/>
+      <c r="D5" s="13">
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:6" ht="24" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="4" t="s">
-        <v>31</v>
-      </c>
-      <c r="B6" s="5" t="s">
+    <row r="6" customHeight="1" spans="1:4">
+      <c r="A6" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="B6" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="C6" s="11"/>
-      <c r="D6" s="10">
+      <c r="C6" s="14"/>
+      <c r="D6" s="13">
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:6" ht="24" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="12"/>
-      <c r="B7" s="13"/>
-      <c r="C7" s="11"/>
-      <c r="D7" s="11"/>
-    </row>
-    <row r="8" spans="1:6" ht="24" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="12"/>
-      <c r="B8" s="13"/>
-      <c r="C8" s="11"/>
-      <c r="D8" s="11"/>
-    </row>
-    <row r="9" spans="1:6" ht="24" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="12"/>
-      <c r="B9" s="13"/>
-      <c r="C9" s="11"/>
-      <c r="D9" s="11"/>
-    </row>
-    <row r="10" spans="1:6" ht="24" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="12"/>
-      <c r="B10" s="13"/>
-      <c r="C10" s="11"/>
-      <c r="D10" s="11"/>
-    </row>
-    <row r="11" spans="1:6" ht="24" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="12"/>
-      <c r="B11" s="13"/>
-      <c r="C11" s="11"/>
-      <c r="D11" s="11"/>
-    </row>
-    <row r="12" spans="1:6" ht="24" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="12"/>
-      <c r="B12" s="13"/>
-      <c r="C12" s="11"/>
-      <c r="D12" s="11"/>
-    </row>
-    <row r="13" spans="1:6" ht="24" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="12"/>
-      <c r="B13" s="13"/>
-      <c r="C13" s="11"/>
-      <c r="D13" s="11"/>
-    </row>
-    <row r="14" spans="1:6" ht="24" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="12"/>
-      <c r="B14" s="13"/>
-      <c r="C14" s="11"/>
-      <c r="D14" s="11"/>
-    </row>
-    <row r="15" spans="1:6" ht="24" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="12"/>
-      <c r="B15" s="13"/>
-      <c r="C15" s="11"/>
-      <c r="D15" s="11"/>
-    </row>
-    <row r="16" spans="1:6" ht="24" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="12"/>
-      <c r="B16" s="13"/>
-      <c r="C16" s="11"/>
-      <c r="D16" s="11"/>
-    </row>
-    <row r="17" spans="1:4" ht="24" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="12"/>
-      <c r="B17" s="13"/>
-      <c r="C17" s="11"/>
-      <c r="D17" s="11"/>
-    </row>
-    <row r="18" spans="1:4" ht="24" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="12"/>
-      <c r="B18" s="13"/>
-      <c r="C18" s="11"/>
-      <c r="D18" s="11"/>
-    </row>
-    <row r="19" spans="1:4" ht="24" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="12"/>
-      <c r="B19" s="13"/>
-      <c r="C19" s="11"/>
-      <c r="D19" s="11"/>
-    </row>
-    <row r="20" spans="1:4" ht="24" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="12"/>
-      <c r="B20" s="13"/>
-      <c r="C20" s="11"/>
-      <c r="D20" s="11"/>
-    </row>
-    <row r="21" spans="1:4" ht="24" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="12"/>
-      <c r="B21" s="13"/>
-      <c r="C21" s="11"/>
-      <c r="D21" s="11"/>
-    </row>
-    <row r="22" spans="1:4" ht="24" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="12"/>
-      <c r="B22" s="13"/>
-      <c r="C22" s="11"/>
-      <c r="D22" s="11"/>
-    </row>
-    <row r="23" spans="1:4" ht="24" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A23" s="12"/>
-      <c r="B23" s="13"/>
-      <c r="C23" s="11"/>
-      <c r="D23" s="11"/>
-    </row>
-    <row r="24" spans="1:4" ht="24" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A24" s="12"/>
-      <c r="B24" s="13"/>
-      <c r="C24" s="11"/>
-      <c r="D24" s="11"/>
-    </row>
-    <row r="25" spans="1:4" ht="24" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A25" s="12"/>
-      <c r="B25" s="13"/>
-      <c r="C25" s="11"/>
-      <c r="D25" s="11"/>
+    <row r="7" customHeight="1" spans="1:4">
+      <c r="A7" s="15"/>
+      <c r="B7" s="16"/>
+      <c r="C7" s="14"/>
+      <c r="D7" s="14"/>
+    </row>
+    <row r="8" customHeight="1" spans="1:4">
+      <c r="A8" s="15"/>
+      <c r="B8" s="16"/>
+      <c r="C8" s="14"/>
+      <c r="D8" s="14"/>
+    </row>
+    <row r="9" customHeight="1" spans="1:4">
+      <c r="A9" s="15"/>
+      <c r="B9" s="16"/>
+      <c r="C9" s="14"/>
+      <c r="D9" s="14"/>
+    </row>
+    <row r="10" customHeight="1" spans="1:4">
+      <c r="A10" s="15"/>
+      <c r="B10" s="16"/>
+      <c r="C10" s="14"/>
+      <c r="D10" s="14"/>
+    </row>
+    <row r="11" customHeight="1" spans="1:4">
+      <c r="A11" s="15"/>
+      <c r="B11" s="16"/>
+      <c r="C11" s="14"/>
+      <c r="D11" s="14"/>
+    </row>
+    <row r="12" customHeight="1" spans="1:4">
+      <c r="A12" s="15"/>
+      <c r="B12" s="16"/>
+      <c r="C12" s="14"/>
+      <c r="D12" s="14"/>
+    </row>
+    <row r="13" customHeight="1" spans="1:4">
+      <c r="A13" s="15"/>
+      <c r="B13" s="16"/>
+      <c r="C13" s="14"/>
+      <c r="D13" s="14"/>
+    </row>
+    <row r="14" customHeight="1" spans="1:4">
+      <c r="A14" s="15"/>
+      <c r="B14" s="16"/>
+      <c r="C14" s="14"/>
+      <c r="D14" s="14"/>
+    </row>
+    <row r="15" customHeight="1" spans="1:4">
+      <c r="A15" s="15"/>
+      <c r="B15" s="16"/>
+      <c r="C15" s="14"/>
+      <c r="D15" s="14"/>
+    </row>
+    <row r="16" customHeight="1" spans="1:4">
+      <c r="A16" s="15"/>
+      <c r="B16" s="16"/>
+      <c r="C16" s="14"/>
+      <c r="D16" s="14"/>
+    </row>
+    <row r="17" customHeight="1" spans="1:4">
+      <c r="A17" s="15"/>
+      <c r="B17" s="16"/>
+      <c r="C17" s="14"/>
+      <c r="D17" s="14"/>
+    </row>
+    <row r="18" customHeight="1" spans="1:4">
+      <c r="A18" s="15"/>
+      <c r="B18" s="16"/>
+      <c r="C18" s="14"/>
+      <c r="D18" s="14"/>
+    </row>
+    <row r="19" customHeight="1" spans="1:4">
+      <c r="A19" s="15"/>
+      <c r="B19" s="16"/>
+      <c r="C19" s="14"/>
+      <c r="D19" s="14"/>
+    </row>
+    <row r="20" customHeight="1" spans="1:4">
+      <c r="A20" s="15"/>
+      <c r="B20" s="16"/>
+      <c r="C20" s="14"/>
+      <c r="D20" s="14"/>
+    </row>
+    <row r="21" customHeight="1" spans="1:4">
+      <c r="A21" s="15"/>
+      <c r="B21" s="16"/>
+      <c r="C21" s="14"/>
+      <c r="D21" s="14"/>
+    </row>
+    <row r="22" customHeight="1" spans="1:4">
+      <c r="A22" s="15"/>
+      <c r="B22" s="16"/>
+      <c r="C22" s="14"/>
+      <c r="D22" s="14"/>
+    </row>
+    <row r="23" customHeight="1" spans="1:4">
+      <c r="A23" s="15"/>
+      <c r="B23" s="16"/>
+      <c r="C23" s="14"/>
+      <c r="D23" s="14"/>
+    </row>
+    <row r="24" customHeight="1" spans="1:4">
+      <c r="A24" s="15"/>
+      <c r="B24" s="16"/>
+      <c r="C24" s="14"/>
+      <c r="D24" s="14"/>
+    </row>
+    <row r="25" customHeight="1" spans="1:4">
+      <c r="A25" s="15"/>
+      <c r="B25" s="16"/>
+      <c r="C25" s="14"/>
+      <c r="D25" s="14"/>
     </row>
   </sheetData>
-  <phoneticPr fontId="10" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <headerFooter/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
+  <dimension ref="A1:C11"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I9" sqref="I9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="18.875" defaultRowHeight="29" customHeight="1" outlineLevelCol="2"/>
+  <cols>
+    <col min="1" max="16383" width="18.875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" customHeight="1" spans="1:3">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="2" customHeight="1" spans="1:3">
+      <c r="A2" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="1"/>
+      <c r="C2" s="1"/>
+    </row>
+    <row r="3" customHeight="1" spans="1:3">
+      <c r="A3" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="4" customHeight="1" spans="1:3">
+      <c r="A4" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="5" customHeight="1" spans="2:3">
+      <c r="B5" t="s">
+        <v>41</v>
+      </c>
+      <c r="C5" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" customHeight="1" spans="2:3">
+      <c r="B6" t="s">
+        <v>42</v>
+      </c>
+      <c r="C6" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" customHeight="1" spans="2:3">
+      <c r="B7" t="s">
+        <v>43</v>
+      </c>
+      <c r="C7" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" customHeight="1" spans="2:3">
+      <c r="B8" t="s">
+        <v>44</v>
+      </c>
+      <c r="C8" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" customHeight="1" spans="2:3">
+      <c r="B9" t="s">
+        <v>45</v>
+      </c>
+      <c r="C9" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" customHeight="1" spans="2:3">
+      <c r="B10" s="3"/>
+      <c r="C10" s="3"/>
+    </row>
+    <row r="11" customHeight="1" spans="2:3">
+      <c r="B11" s="3"/>
+      <c r="C11" s="3"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <headerFooter/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
update TDML title phaser
</commit_message>
<xml_diff>
--- a/Luban/Config/Datas/Config.xlsx
+++ b/Luban/Config/Datas/Config.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="28125" windowHeight="12540" activeTab="3"/>
+    <workbookView windowWidth="28125" windowHeight="12540"/>
   </bookViews>
   <sheets>
     <sheet name="UIConfig" sheetId="1" r:id="rId1"/>
@@ -167,7 +167,7 @@
     <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
-  <fonts count="24">
+  <fonts count="23">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -185,13 +185,6 @@
     <font>
       <sz val="11"/>
       <color rgb="FF9C0006"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
       <name val="宋体"/>
       <charset val="134"/>
       <scheme val="minor"/>
@@ -687,10 +680,10 @@
     <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="8" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="8" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -699,7 +692,7 @@
     <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -708,24 +701,27 @@
     <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="3" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="3" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
@@ -735,97 +731,94 @@
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="15" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="15" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="16" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="15" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="15" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="16" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="22" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -835,7 +828,7 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="31" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="7" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
@@ -847,21 +840,21 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="31" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="4" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="31" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="5" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="7" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="3" fontId="4" fillId="6" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="3" fontId="3" fillId="6" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
@@ -873,8 +866,8 @@
     <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="31" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="7" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="31" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="7" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="49">
     <cellStyle name="常规" xfId="0" builtinId="0"/>
@@ -1225,8 +1218,8 @@
   <sheetPr/>
   <dimension ref="A1:F13"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1:D13"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="24" customHeight="1" outlineLevelCol="5"/>
@@ -1793,7 +1786,7 @@
   <sheetPr/>
   <dimension ref="A1:C11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="I9" sqref="I9"/>
     </sheetView>
   </sheetViews>

</xml_diff>